<commit_message>
add part buy and sale product
</commit_message>
<xml_diff>
--- a/GUI/bin/Debug/Output.xlsx
+++ b/GUI/bin/Debug/Output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="15">
   <si>
     <t>ID</t>
   </si>
@@ -23,28 +23,37 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>NV000001</t>
-  </si>
-  <si>
-    <t>Admin</t>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>KV000001</t>
+  </si>
+  <si>
+    <t>Miền Nam</t>
+  </si>
+  <si>
+    <t>KV000002</t>
+  </si>
+  <si>
+    <t>hieu</t>
+  </si>
+  <si>
+    <t>KV000003</t>
+  </si>
+  <si>
+    <t>Miền Trung</t>
+  </si>
+  <si>
+    <t>KV000004</t>
+  </si>
+  <si>
+    <t>Đông Nam Bộ</t>
+  </si>
+  <si>
+    <t>SP00005</t>
+  </si>
+  <si>
+    <t>Trung Du</t>
   </si>
   <si>
     <t>Created with a trial version of Syncfusion Essential XlsIO</t>
@@ -157,7 +166,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -165,15 +174,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.84765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.84765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.84765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.84765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -183,28 +189,48 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -229,11 +255,11 @@
   <sheetData>
     <row r="10" spans="1:1" ht="25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vfmvqZ+QuM69rDPhQAvmyN8poQBGXQSvzT8WZVPkFc761wMx0WVMcarM3g0l1OZx6XlNFqFKzouRSN/8pQQwew==" saltValue="L8vJyRh/OXJ90BVGY5TgyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" pivotTables="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rPkS5peNAPre8vcPg/m1/VTJQHWdT8GIidcgBGMkYenUYPjjDJ+nw27PJmIlXbVWZc+erYUbg95p7MYksIjK6Q==" saltValue="UTvDlUnbtIQCNAJtaUI5jA==" spinCount="100000" sheet="1" objects="1" scenarios="1" pivotTables="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
   <extLst/>

</xml_diff>

<commit_message>
add buy and sell product
</commit_message>
<xml_diff>
--- a/GUI/bin/Debug/Output.xlsx
+++ b/GUI/bin/Debug/Output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16" count="17">
   <si>
     <t>ID</t>
   </si>
@@ -50,10 +50,16 @@
     <t>Đông Nam Bộ</t>
   </si>
   <si>
-    <t>SP00005</t>
+    <t>KV000005</t>
   </si>
   <si>
     <t>Trung Du</t>
+  </si>
+  <si>
+    <t>KV000006</t>
+  </si>
+  <si>
+    <t>Tây Nam Bộ</t>
   </si>
   <si>
     <t>Created with a trial version of Syncfusion Essential XlsIO</t>
@@ -166,7 +172,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -233,6 +239,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
@@ -255,11 +269,11 @@
   <sheetData>
     <row r="10" spans="1:1" ht="25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rPkS5peNAPre8vcPg/m1/VTJQHWdT8GIidcgBGMkYenUYPjjDJ+nw27PJmIlXbVWZc+erYUbg95p7MYksIjK6Q==" saltValue="UTvDlUnbtIQCNAJtaUI5jA==" spinCount="100000" sheet="1" objects="1" scenarios="1" pivotTables="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4Ul5jnN9VtzOdHZWHFz15lnJWJgYefbN9kBjYzi7eX0+VE+ele4ncmk8Nv1PfpjTWBfT3wWtxDmrkUx5DOZcZQ==" saltValue="Mx61Am4SOecelck2bPISgA==" spinCount="100000" sheet="1" objects="1" scenarios="1" pivotTables="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
   <extLst/>

</xml_diff>